<commit_message>
Updated development time with Dana's measurements
</commit_message>
<xml_diff>
--- a/Development/Consolidated Orius Development JB2020.xlsx
+++ b/Development/Consolidated Orius Development JB2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Development Data JB2020" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="186">
   <si>
     <t>JB2020 Notes</t>
   </si>
@@ -580,7 +580,13 @@
     <t>Fate (A = adult, D = dead, E = escaped, U = unknown not included)</t>
   </si>
   <si>
-    <t>missing tibia length</t>
+    <t>was missing tibia length, Dana re-measured and sexed as M</t>
+  </si>
+  <si>
+    <t>Dana re-measured and sexed as F (was previously sexed as M)</t>
+  </si>
+  <si>
+    <t>Dana re-measured and sexed as F</t>
   </si>
 </sst>
 </file>
@@ -8899,7 +8905,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E23" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="22">
     <pivotField axis="axisRow" showAll="0">
@@ -9312,9 +9318,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V338"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+    <sheetView zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L284" sqref="L284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25441,7 +25447,7 @@
         <v/>
       </c>
       <c r="R258" s="4" t="e">
-        <f t="shared" ref="R258:R321" si="88">SUM(M258:Q258)</f>
+        <f t="shared" ref="R258:R316" si="88">SUM(M258:Q258)</f>
         <v>#VALUE!</v>
       </c>
       <c r="S258" s="4">
@@ -26743,7 +26749,10 @@
         <v>29</v>
       </c>
       <c r="J279" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="L279" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="M279" s="4">
         <f>1/2</f>
@@ -26771,15 +26780,15 @@
       </c>
       <c r="S279" s="4" t="str">
         <f t="shared" si="89"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="T279" s="4">
         <f t="shared" si="90"/>
         <v>0</v>
       </c>
-      <c r="U279" s="4">
+      <c r="U279" s="4" t="str">
         <f t="shared" si="91"/>
-        <v>0</v>
+        <v>Dana re-measured and sexed as F (was previously sexed as M)</v>
       </c>
       <c r="V279" s="4" t="s">
         <v>107</v>
@@ -27007,6 +27016,9 @@
       <c r="J283" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="L283" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="M283" s="4">
         <f t="shared" si="97"/>
         <v>1</v>
@@ -27039,9 +27051,9 @@
         <f t="shared" si="90"/>
         <v>0</v>
       </c>
-      <c r="U283" s="4">
+      <c r="U283" s="4" t="str">
         <f t="shared" si="91"/>
-        <v>0</v>
+        <v>was missing tibia length, Dana re-measured and sexed as M</v>
       </c>
       <c r="V283" s="4" t="s">
         <v>107</v>
@@ -27323,6 +27335,9 @@
       <c r="J288" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="L288" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="M288" s="4">
         <f t="shared" si="99"/>
         <v>1</v>
@@ -27355,9 +27370,9 @@
         <f t="shared" si="90"/>
         <v>0</v>
       </c>
-      <c r="U288" s="4">
+      <c r="U288" s="4" t="str">
         <f t="shared" si="91"/>
-        <v>0</v>
+        <v>was missing tibia length, Dana re-measured and sexed as M</v>
       </c>
       <c r="V288" s="4" t="s">
         <v>107</v>
@@ -27914,6 +27929,9 @@
       <c r="J297" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="L297" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="M297" s="4">
         <f t="shared" si="99"/>
         <v>1</v>
@@ -27946,9 +27964,9 @@
         <f t="shared" si="90"/>
         <v>0</v>
       </c>
-      <c r="U297" s="4">
+      <c r="U297" s="4" t="str">
         <f t="shared" si="91"/>
-        <v>0</v>
+        <v>Dana re-measured and sexed as F</v>
       </c>
       <c r="V297" s="4" t="s">
         <v>107</v>
@@ -29710,9 +29728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30586,7 +30604,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>2</v>
       </c>
@@ -30604,7 +30622,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>2</v>
       </c>
@@ -30622,7 +30640,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>2</v>
       </c>
@@ -30640,7 +30658,7 @@
         <v>0.44000000000000006</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>2</v>
       </c>
@@ -30658,7 +30676,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>2</v>
       </c>
@@ -30676,7 +30694,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>2</v>
       </c>
@@ -30694,7 +30712,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="6">
         <v>2</v>
       </c>
@@ -30712,7 +30730,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>2</v>
       </c>
@@ -30730,7 +30748,7 @@
         <v>0.42000000000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>2</v>
       </c>
@@ -30748,7 +30766,7 @@
         <v>0.55999999999999994</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>2</v>
       </c>
@@ -30765,8 +30783,11 @@
         <f t="shared" si="9"/>
         <v>0.52</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F58" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>2</v>
       </c>
@@ -30784,7 +30805,7 @@
         <v>0.44000000000000006</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
         <v>2</v>
       </c>
@@ -30802,7 +30823,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>2</v>
       </c>
@@ -30820,7 +30841,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>2</v>
       </c>
@@ -30838,7 +30859,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>2</v>
       </c>
@@ -30856,7 +30877,7 @@
         <v>0.55999999999999994</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>2</v>
       </c>
@@ -30903,11 +30924,14 @@
         <v>3</v>
       </c>
       <c r="D66" s="6">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="E66" s="6">
         <f t="shared" si="9"/>
-        <v>0.54</v>
+        <v>0.52</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -31010,9 +31034,12 @@
       <c r="C72" s="1">
         <v>8</v>
       </c>
+      <c r="D72" s="1">
+        <v>2.6</v>
+      </c>
       <c r="E72">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>183</v>
@@ -31028,10 +31055,12 @@
       <c r="C73" s="6">
         <v>13</v>
       </c>
-      <c r="D73" s="6"/>
+      <c r="D73" s="6">
+        <v>2.7</v>
+      </c>
       <c r="E73">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>183</v>

</xml_diff>